<commit_message>
Rail and aviation edits
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/trans/avlo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF917F2-0352-6547-A722-24697CAA4973}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D811A2-6692-4FAB-8E52-3642C77463EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="3795" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>weighted value, adjusted for number of train cars per locomotive</t>
+  </si>
+  <si>
+    <t>Assumption - train cars per locomotive</t>
   </si>
 </sst>
 </file>
@@ -1867,14 +1870,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="85.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2133,17 +2136,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.6640625" customWidth="1"/>
+    <col min="1" max="1" width="73.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="102.33203125" customWidth="1"/>
+    <col min="3" max="3" width="102.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2300,364 +2303,369 @@
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B23" s="12">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
-        <v>5914</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>5914</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="6">
-        <f>B24/B23</f>
+      <c r="B26" s="6">
+        <f>B25/B24</f>
         <v>155.63157894736841</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B27" s="12">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="6">
-        <v>16805</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6">
-        <v>2196</v>
+        <v>16805</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="6">
-        <v>11129</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="6">
-        <v>685</v>
+        <v>11129</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6">
-        <v>90</v>
+        <v>685</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="6">
-        <v>337</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="6">
-        <f>B27/B30</f>
-        <v>24.532846715328468</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="6">
-        <f t="shared" ref="B34:B35" si="0">B28/B31</f>
-        <v>24.4</v>
+        <f>B28/B31</f>
+        <v>24.532846715328468</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="6">
+        <f t="shared" ref="B35:B36" si="0">B29/B32</f>
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B36" s="6">
         <f t="shared" si="0"/>
         <v>33.023738872403563</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16">
-      <c r="A36" s="10" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="6">
-        <f>(B25*B24+B33*B27+B34*B28+B35*B29)/SUM(B24,B27:B29)</f>
+      <c r="B37" s="6">
+        <f>(B26*B25+B34*B28+B35*B29+B36*B30)/SUM(B25,B28:B30)*B22</f>
+        <v>486.56731685074101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="6">
+        <f>B37/10</f>
         <v>48.656731685074099</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16">
-      <c r="A37" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" s="6">
-        <f>B36/10</f>
-        <v>4.8656731685074099</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B40" s="4">
         <v>2005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="15">
-        <v>2967</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="15">
-        <v>100</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B42" s="15">
-        <v>27876</v>
-      </c>
-      <c r="C42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="15">
+        <v>27876</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B44" s="15">
         <v>4151</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="B44" s="15"/>
-      <c r="C44" t="s">
+    <row r="45" spans="1:3">
+      <c r="B45" s="15"/>
+      <c r="C45" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="15">
-        <v>6614973</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="15">
-        <v>5727512</v>
+        <v>6614973</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B47" s="15">
-        <v>44777151</v>
+        <v>5727512</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="15">
+        <v>44777151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B49" s="15">
         <v>12172542</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="B49" s="15"/>
-    </row>
     <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="15">
-        <f>B45/B40</f>
-        <v>2229.5156723963601</v>
-      </c>
+      <c r="B50" s="15"/>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="15">
         <f>B46/B41</f>
-        <v>57275.12</v>
+        <v>2229.5156723963601</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B52" s="15">
-        <f t="shared" ref="B52:B53" si="1">B47/B42</f>
-        <v>1606.2975678002583</v>
+        <f>B47/B42</f>
+        <v>57275.12</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="15">
+        <f t="shared" ref="B53:B54" si="1">B48/B43</f>
+        <v>1606.2975678002583</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B54" s="15">
         <f t="shared" si="1"/>
         <v>2932.4360395085523</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="B54" s="15"/>
-    </row>
     <row r="55" spans="1:2">
-      <c r="A55" t="s">
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="15">
-        <f>SUMPRODUCT(B40:B43,B50:B53)/SUM(B40:B43)</f>
+      <c r="B56" s="15">
+        <f>SUMPRODUCT(B41:B44,B51:B54)/SUM(B41:B44)</f>
         <v>1974.4736422180429</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="B56" s="6"/>
-    </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="4" t="s">
+      <c r="B57" s="6"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B58" s="13">
         <v>2007</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>55</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>13611</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="11" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B60" s="11">
         <v>17287</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16">
-      <c r="A60" s="10" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="7">
-        <f>B59/B58</f>
+      <c r="B61" s="7">
+        <f>B60/B59</f>
         <v>1.2700756740871355</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="10"/>
-    </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="10"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B63" s="4">
         <v>2007</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="11">
-        <v>1670994</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="6">
-        <v>2640170</v>
+        <v>59</v>
+      </c>
+      <c r="B64" s="11">
+        <v>1670994</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="6">
+        <v>2640170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="7">
-        <f>B64/B63</f>
+      <c r="B66" s="7">
+        <f>B65/B64</f>
         <v>1.579999688807979</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C66" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="B66" s="6"/>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" s="6"/>
     </row>
-    <row r="69" spans="1:3">
-      <c r="B69" s="9"/>
+    <row r="68" spans="1:3">
+      <c r="B68" s="6"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B36" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2668,17 +2676,17 @@
   </sheetPr>
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="48">
+    <row r="1" spans="1:37" ht="45">
       <c r="A1" s="19" t="s">
         <v>111</v>
       </c>
@@ -3242,148 +3250,148 @@
         <v>15</v>
       </c>
       <c r="B5" s="9">
-        <f>'BTS NTS Modal Profile Data'!B37</f>
-        <v>4.8656731685074099</v>
+        <f>'BTS NTS Modal Profile Data'!B38</f>
+        <v>48.656731685074099</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="1"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AE5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AG5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AH5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AI5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AJ5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
       <c r="AK5" s="7">
         <f t="shared" si="0"/>
-        <v>4.8656731685074099</v>
+        <v>48.656731685074099</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -3539,7 +3547,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="7">
-        <f>'BTS NTS Modal Profile Data'!B60</f>
+        <f>'BTS NTS Modal Profile Data'!B61</f>
         <v>1.2700756740871355</v>
       </c>
       <c r="C7" s="7">
@@ -3695,14 +3703,16 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="32">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="45">
       <c r="A1" s="19" t="s">
         <v>112</v>
       </c>
@@ -4395,7 +4405,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="6">
-        <f>'BTS NTS Modal Profile Data'!B55</f>
+        <f>'BTS NTS Modal Profile Data'!B56</f>
         <v>1974.4736422180429</v>
       </c>
       <c r="C6" s="6">

</xml_diff>